<commit_message>
Testing how to Commit and Push to GitHub. Solving a problem with Syng and Push.
</commit_message>
<xml_diff>
--- a/Logs/1st Week Logs.xlsx
+++ b/Logs/1st Week Logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17408543-FCD4-4BF4-B68A-4D983A481E0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E69EC8-9C99-4594-8032-3B5E88EB92EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -956,7 +956,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1258,9 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <v>10</v>
+      </c>
       <c r="G15" s="14"/>
       <c r="H15" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Windows Forms Lecture (Done)
</commit_message>
<xml_diff>
--- a/Logs/1st Week Logs.xlsx
+++ b/Logs/1st Week Logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE77B4D8-CAFB-40C9-B333-8C7D184D64D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943B9ECE-9879-403C-8D5D-B235045701B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -956,7 +956,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,13 +1257,17 @@
       <c r="D15" s="16">
         <v>0.67708333333333337</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="16">
+        <v>0.86805555555555547</v>
+      </c>
       <c r="F15" s="4">
-        <v>10</v>
-      </c>
-      <c r="G15" s="14"/>
+        <v>50</v>
+      </c>
+      <c r="G15" s="14">
+        <v>225</v>
+      </c>
       <c r="H15" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>22</v>
@@ -1329,7 +1333,7 @@
       </c>
       <c r="G20" s="20">
         <f>SUM(G8:G19)</f>
-        <v>985</v>
+        <v>1210</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>

</xml_diff>